<commit_message>
Commit for 3/20/2013 work on Clue Game Players. Implemented two tests in GameSetupTests
</commit_message>
<xml_diff>
--- a/ClueBoardTwo/Clue Board.xlsx
+++ b/ClueBoardTwo/Clue Board.xlsx
@@ -224,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -232,11 +232,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -246,12 +261,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +572,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +583,7 @@
     <col min="27" max="27" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -586,7 +602,7 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -714,10 +730,10 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="Z2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="10"/>
+      <c r="AA2" s="11"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -959,7 +975,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1039,8 +1055,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1325,7 +1341,7 @@
       <c r="O10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="Q10" s="4" t="s">
@@ -1696,7 +1712,7 @@
       <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="9" t="s">
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -2415,89 +2431,89 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Started Clue Game Players Part II. Implemented pickLocation(), checkAccusation(), loadPeopleFile(), and part of loadCardFile()
</commit_message>
<xml_diff>
--- a/ClueBoardTwo/Clue Board.xlsx
+++ b/ClueBoardTwo/Clue Board.xlsx
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -262,12 +262,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +573,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +603,7 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -617,7 +618,7 @@
       <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -638,7 +639,7 @@
       <c r="R1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -730,10 +731,10 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Z2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="11"/>
+      <c r="AA2" s="12"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1056,7 +1057,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1375,7 +1376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +1456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1523,7 @@
       <c r="V12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="X12">
@@ -1693,7 +1694,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1767,8 +1768,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1841,7 +1842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1982,7 +1983,7 @@
       <c r="V18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="7" t="s">
+      <c r="W18" s="14" t="s">
         <v>2</v>
       </c>
       <c r="X18">
@@ -2211,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -2301,7 +2302,7 @@
       <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="10" t="s">
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -2331,7 +2332,7 @@
       <c r="O23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="7" t="s">
+      <c r="P23" s="14" t="s">
         <v>2</v>
       </c>
       <c r="Q23" s="4" t="s">
@@ -2431,89 +2432,89 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>